<commit_message>
Finalizo las pruebas del ejercicio del algoritmo que coordina.
</commit_message>
<xml_diff>
--- a/2da parte/El algoritmo coordinador/Especificaciones/Agregar proyecto.xlsx
+++ b/2da parte/El algoritmo coordinador/Especificaciones/Agregar proyecto.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\Source\Repos\sm.vb.diseno-con-pruebas-unitarias\2da parte\Composicion de algoritmos\Especificaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\Source\Repos\sm.vb.diseno-con-pruebas-unitarias\2da parte\El algoritmo coordinador\Especificaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8925" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8925" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="6" state="hidden" r:id="rId1"/>
     <sheet name="Cómo programarlo" sheetId="7" state="hidden" r:id="rId2"/>
-    <sheet name="Creacion de un nuevo proyecto" sheetId="4" r:id="rId3"/>
+    <sheet name="Valide el nuevo proyecto" sheetId="8" r:id="rId3"/>
+    <sheet name="Genere el proyecto por crear" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="142">
   <si>
     <t>Entonces</t>
   </si>
@@ -453,6 +454,75 @@
   </si>
   <si>
     <t>Además, siempre utilice las palabras del negocio, no palabras técnicas o abreviaturas que no sean comunes.</t>
+  </si>
+  <si>
+    <t>Valide el nuevo proyecto</t>
+  </si>
+  <si>
+    <t>Dados</t>
+  </si>
+  <si>
+    <t>los proyectos existentes</t>
+  </si>
+  <si>
+    <t>Proyecto 1</t>
+  </si>
+  <si>
+    <t>Proyecto 2</t>
+  </si>
+  <si>
+    <t>se indica si &lt;es valido o no&gt;</t>
+  </si>
+  <si>
+    <t>se valida el nuevo proyecto con nombre &lt;nombre&gt; y la fecha de inicio es &lt;fecha de inicio&gt;</t>
+  </si>
+  <si>
+    <t>Ejemplos</t>
+  </si>
+  <si>
+    <t>Es valido o no</t>
+  </si>
+  <si>
+    <t>El nombre es requerido</t>
+  </si>
+  <si>
+    <t>Son validos</t>
+  </si>
+  <si>
+    <t>Proyecto asombroso</t>
+  </si>
+  <si>
+    <t>Es válido</t>
+  </si>
+  <si>
+    <t>El nombre tiene un tamaño máximo de 200 caracteres</t>
+  </si>
+  <si>
+    <t>El nombre no puede contener solamente espacios en blanco</t>
+  </si>
+  <si>
+    <t>El nombre sólo puede contener letras y números</t>
+  </si>
+  <si>
+    <t>El nombre debe ser único</t>
+  </si>
+  <si>
+    <t>La fecha de inicio es requerida</t>
+  </si>
+  <si>
+    <t>nula</t>
+  </si>
+  <si>
+    <t>Es inválido</t>
+  </si>
+  <si>
+    <t>"1234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901"</t>
+  </si>
+  <si>
+    <t>"    "</t>
+  </si>
+  <si>
+    <t>Hola-Mundo</t>
   </si>
 </sst>
 </file>
@@ -882,6 +952,29 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A12:D19" totalsRowShown="0">
+  <autoFilter ref="A12:D19"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Ejemplo"/>
+    <tableColumn id="2" name="Nombre"/>
+    <tableColumn id="3" name="Fecha de inicio"/>
+    <tableColumn id="4" name="Es valido o no"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:B6" totalsRowShown="0">
+  <autoFilter ref="B4:B6"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nombre"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A7:B10" totalsRowShown="0">
   <autoFilter ref="A7:B10"/>
   <tableColumns count="2">
@@ -1951,11 +2044,203 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="4">
+        <v>43399</v>
+      </c>
+      <c r="D13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="4">
+        <v>43399</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="4">
+        <v>43399</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="4">
+        <v>43399</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="4">
+        <v>43399</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="4">
+        <v>43399</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>